<commit_message>
generates GH pages! removes temporary elements!
</commit_message>
<xml_diff>
--- a/schema_derivatives/GSC_MIxS_6.form.xlsx
+++ b/schema_derivatives/GSC_MIxS_6.form.xlsx
@@ -5721,222 +5721,222 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>collection_date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>tax_class</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>geo_loc_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nucl_acid_ext</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>lib_reads_seqd</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>lat_lon</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>env_local_scale</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>samp_name</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>elev</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>sim_search_meth</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>samp_taxon_id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>samp_mat_process</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>lib_screen</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>seq_meth</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>samp_size</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>source_mat_id</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>mid</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>assembly_qual</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>size_frac</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>env_medium</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>samp_collect_device</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>feat_pred</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>lib_size</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>env_broad_scale</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>lib_vector</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>assembly_name</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>samp_vol_we_dna_ext</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>adapters</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>number_contig</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>neg_cont_type</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>nucl_acid_amp</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>alt</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>lib_layout</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
           <t>annot</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>project_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>env_local_scale</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>tax_class</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>experimental_factor</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>pos_cont_type</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>ref_biomaterial</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
         <is>
           <t>assembly_software</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>size_frac</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>sim_search_meth</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>rel_to_oxygen</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>ref_db</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
         <is>
           <t>samp_collect_method</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>experimental_factor</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>pos_cont_type</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>lat_lon</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>lib_size</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>samp_taxon_id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>neg_cont_type</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>mid</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>seq_meth</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>number_contig</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>samp_size</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>feat_pred</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>lib_vector</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>depth</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>ref_db</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>samp_mat_process</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>adapters</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>lib_layout</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>geo_loc_name</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>nucl_acid_amp</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>source_mat_id</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>samp_collect_device</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>collection_date</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>lib_screen</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>ref_biomaterial</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>elev</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>rel_to_oxygen</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>nucl_acid_ext</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
-        <is>
-          <t>assembly_name</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>samp_name</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>assembly_qual</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>env_medium</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>samp_vol_we_dna_ext</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>alt</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>temp</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>lib_reads_seqd</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>env_broad_scale</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
@@ -6202,13 +6202,13 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AG2:AG1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"DNA-free PCR mix,distilled water,empty collection device,empty collection tube,phosphate buffer,sterile swab,sterile syringe"</formula1>
     </dataValidation>
-    <dataValidation sqref="Y2:Y1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AJ2:AJ1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"other,paired,single,vector"</formula1>
     </dataValidation>
-    <dataValidation sqref="AH2:AH1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="AP2:AP1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"aerobe,anaerobe,facultative,microaerophilic,microanaerobe,obligate aerobe,obligate anaerobe"</formula1>
     </dataValidation>
     <dataValidation sqref="BB2:BB1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">

</xml_diff>

<commit_message>
more write_mixs_linkml param updates
</commit_message>
<xml_diff>
--- a/schema_derivatives/GSC_MIxS_6.form.xlsx
+++ b/schema_derivatives/GSC_MIxS_6.form.xlsx
@@ -5721,222 +5721,222 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>ref_biomaterial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>samp_collect_method</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sim_search_meth</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>project_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>elev</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>samp_collect_device</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>tax_class</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mid</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>adapters</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>neg_cont_type</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>assembly_name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>samp_taxon_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>samp_name</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>lib_reads_seqd</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>assembly_qual</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>geo_loc_name</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>annot</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>collection_date</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>size_frac</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>lib_layout</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>nucl_acid_ext</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
         <is>
           <t>rel_to_oxygen</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>lat_lon</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>env_local_scale</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>samp_vol_we_dna_ext</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>assembly_software</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>samp_size</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>temp</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>samp_mat_process</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>ref_db</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>nucl_acid_amp</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>feat_pred</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>env_broad_scale</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>lib_screen</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>env_medium</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>number_contig</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
         <is>
           <t>pos_cont_type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>tax_class</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>lat_lon</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>sim_search_meth</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>size_frac</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>env_medium</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>assembly_qual</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>ref_db</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>samp_collect_device</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>nucl_acid_amp</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>neg_cont_type</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>samp_name</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>annot</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>lib_vector</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
         <is>
           <t>source_mat_id</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>env_broad_scale</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>ref_biomaterial</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>project_name</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>collection_date</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>samp_vol_we_dna_ext</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>temp</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>experimental_factor</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>seq_meth</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>adapters</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>env_local_scale</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>elev</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>assembly_software</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>lib_reads_seqd</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>feat_pred</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>lib_layout</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>lib_vector</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>number_contig</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>samp_mat_process</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>lib_screen</t>
-        </is>
-      </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>alt</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
         <is>
           <t>lib_size</t>
-        </is>
-      </c>
-      <c r="AK1" t="inlineStr">
-        <is>
-          <t>nucl_acid_ext</t>
-        </is>
-      </c>
-      <c r="AL1" t="inlineStr">
-        <is>
-          <t>assembly_name</t>
-        </is>
-      </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>alt</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>geo_loc_name</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>mid</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>samp_size</t>
-        </is>
-      </c>
-      <c r="AQ1" t="inlineStr">
-        <is>
-          <t>depth</t>
-        </is>
-      </c>
-      <c r="AR1" t="inlineStr">
-        <is>
-          <t>samp_collect_method</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
@@ -6202,14 +6202,14 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"DNA-free PCR mix,distilled water,empty collection device,empty collection tube,phosphate buffer,sterile swab,sterile syringe"</formula1>
+    </dataValidation>
+    <dataValidation sqref="U2:U1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"other,paired,single,vector"</formula1>
+    </dataValidation>
+    <dataValidation sqref="W2:W1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"aerobe,anaerobe,facultative,microaerophilic,microanaerobe,obligate aerobe,obligate anaerobe"</formula1>
-    </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"DNA-free PCR mix,distilled water,empty collection device,empty collection tube,phosphate buffer,sterile swab,sterile syringe"</formula1>
-    </dataValidation>
-    <dataValidation sqref="AE2:AE1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"other,paired,single,vector"</formula1>
     </dataValidation>
     <dataValidation sqref="BB2:BB1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"chisel,cutting disc,disc plough,drill,mouldboard,ridge till,strip tillage,tined,zonal tillage"</formula1>

</xml_diff>